<commit_message>
now supporting attribute comobo options
</commit_message>
<xml_diff>
--- a/template-data-import/template.xlsx
+++ b/template-data-import/template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27417"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="27760" windowHeight="14360" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="27760" windowHeight="14360" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DATA_ELEMENT_A" sheetId="1" r:id="rId1"/>
@@ -184,7 +184,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="38">
   <si>
     <t>Org Unit</t>
   </si>
@@ -295,6 +295,9 @@
   </si>
   <si>
     <t>Data Element A</t>
+  </si>
+  <si>
+    <t>Project Code (attribute option)</t>
   </si>
 </sst>
 </file>
@@ -426,8 +429,8 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
+      <sheetName val="Home"/>
       <sheetName val="Instructions"/>
-      <sheetName val="Home"/>
       <sheetName val="TX"/>
       <sheetName val="HTS_FACILITY"/>
       <sheetName val="HTS_COMMUNITY"/>
@@ -446,318 +449,6 @@
         <row r="1">
           <cell r="F1" t="str">
             <v>Site Name</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="F2" t="str">
-            <v>1Div Military HOSPITAL</v>
-          </cell>
-          <cell r="G2" t="str">
-            <v>MIL_UGA800_1005533_17855</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="F3" t="str">
-            <v>407 Brigade HC III</v>
-          </cell>
-          <cell r="G3" t="str">
-            <v>MIL_UGA800_1004630_17855</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="F4" t="str">
-            <v>5Th Military Division HOSPITAL</v>
-          </cell>
-          <cell r="G4" t="str">
-            <v>MIL_UGA800_1004985_17855</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="F5" t="str">
-            <v>Bagezza subcounty</v>
-          </cell>
-          <cell r="G5" t="str">
-            <v>MIL_UGA800_1006728_17855</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="F6" t="str">
-            <v>Bardege division</v>
-          </cell>
-          <cell r="G6" t="str">
-            <v>MIL_UGA800_1006176_17855</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="F7" t="str">
-            <v>Bombo General Military HOSPITAL</v>
-          </cell>
-          <cell r="G7" t="str">
-            <v>MIL_UGA800_1003805_17855</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="F8" t="str">
-            <v>Bombo Town council</v>
-          </cell>
-          <cell r="G8" t="str">
-            <v>MIL_UGA800_1006236_17855</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="F9" t="str">
-            <v>Central division Masindi</v>
-          </cell>
-          <cell r="G9" t="str">
-            <v>MIL_UGA800_1006576_17855</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="F10" t="str">
-            <v>Entebbe Division A</v>
-          </cell>
-          <cell r="G10" t="str">
-            <v>MIL_UGA800_1006410_17855</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="F11" t="str">
-            <v>Gaddafi Health Centre III</v>
-          </cell>
-          <cell r="G11" t="str">
-            <v>MIL_UGA800_1001300_17855</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="F12" t="str">
-            <v>Gulu Military Hospital</v>
-          </cell>
-          <cell r="G12" t="str">
-            <v>MIL_UGA800_1000839_17855</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="F13" t="str">
-            <v>Kabamba/Kabamba Barracks Health Centre III</v>
-          </cell>
-          <cell r="G13" t="str">
-            <v>MIL_UGA800_1004503_17855</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="F14" t="str">
-            <v>Kakiri Town council</v>
-          </cell>
-          <cell r="G14" t="str">
-            <v>MIL_UGA800_1006198_17855</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="F15" t="str">
-            <v>Kakoba division</v>
-          </cell>
-          <cell r="G15" t="str">
-            <v>MIL_UGA800_1006251_17855</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="F16" t="str">
-            <v>Kapeeka Subcounty</v>
-          </cell>
-          <cell r="G16" t="str">
-            <v>MIL_UGA800_1006469_17855</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="F17" t="str">
-            <v>Katabi Military Health Centre III</v>
-          </cell>
-          <cell r="G17" t="str">
-            <v>MIL_UGA800_1005504_17855</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="F18" t="str">
-            <v>Kaweweta Health Centre II</v>
-          </cell>
-          <cell r="G18" t="str">
-            <v>MIL_UGA800_1004655_17855</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="F19" t="str">
-            <v>Kinyogoga Subcounty</v>
-          </cell>
-          <cell r="G19" t="str">
-            <v>MIL_UGA800_1006187_17855</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="F20" t="str">
-            <v>Kyankwanzi subcounty</v>
-          </cell>
-          <cell r="G20" t="str">
-            <v>MIL_UGA800_1006657_17855</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="F21" t="str">
-            <v>Lira Barracks HC III</v>
-          </cell>
-          <cell r="G21" t="str">
-            <v>MIL_UGA800_1005545_17855</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="F22" t="str">
-            <v>Luwunga Barracks</v>
-          </cell>
-          <cell r="G22" t="str">
-            <v>MIL_UGA800_1007783_17855</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="F23" t="str">
-            <v>Lwampanga Subcounty</v>
-          </cell>
-          <cell r="G23" t="str">
-            <v>MIL_UGA800_1006249_17855</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="F24" t="str">
-            <v>Makindye Barracks Health Centre III</v>
-          </cell>
-          <cell r="G24" t="str">
-            <v>MIL_UGA800_1002161_17855</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="F25" t="str">
-            <v>Makindye Division</v>
-          </cell>
-          <cell r="G25" t="str">
-            <v>MIL_UGA800_1006904_17855</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="F26" t="str">
-            <v>Masindi Military/Army Barracks Health Centre IV</v>
-          </cell>
-          <cell r="G26" t="str">
-            <v>MIL_UGA800_1004045_17855</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="F27" t="str">
-            <v>Mbuya Military clinic(MOD garrison)</v>
-          </cell>
-          <cell r="G27" t="str">
-            <v>MIL_UGA800_1002490_17855</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="F28" t="str">
-            <v>Moroto Army Health Centre III</v>
-          </cell>
-          <cell r="G28" t="str">
-            <v>MIL_UGA800_1004347_17855</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="F29" t="str">
-            <v>Mpumudde/Kimaka Division</v>
-          </cell>
-          <cell r="G29" t="str">
-            <v>MIL_UGA800_1006989_17855</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="F30" t="str">
-            <v>Mubende Rehabilitation Centre Health Centre III</v>
-          </cell>
-          <cell r="G30" t="str">
-            <v>MIL_UGA800_1004498_17855</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="F31" t="str">
-            <v>Mubende Town council</v>
-          </cell>
-          <cell r="G31" t="str">
-            <v>MIL_UGA800_1006725_17855</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="F32" t="str">
-            <v>Muhooti Baracks HC II</v>
-          </cell>
-          <cell r="G32" t="str">
-            <v>MIL_UGA800_1004822_17855</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="F33" t="str">
-            <v>Nakasongola Military HOSPITAL</v>
-          </cell>
-          <cell r="G33" t="str">
-            <v>MIL_UGA800_1004694_17855</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="F34" t="str">
-            <v>Nakawa Division</v>
-          </cell>
-          <cell r="G34" t="str">
-            <v>MIL_UGA800_1006958_17855</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="F35" t="str">
-            <v>Rubongi Military HOSPITAL</v>
-          </cell>
-          <cell r="G35" t="str">
-            <v>MIL_UGA800_1005479_17855</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="F36" t="str">
-            <v>Rubongi subcounty</v>
-          </cell>
-          <cell r="G36" t="str">
-            <v>MIL_UGA800_1006415_17855</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="F37" t="str">
-            <v>Rupa Subcounty</v>
-          </cell>
-          <cell r="G37" t="str">
-            <v>MIL_UGA800_1006535_17855</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="F38" t="str">
-            <v xml:space="preserve">Singo HC II </v>
-          </cell>
-          <cell r="G38" t="str">
-            <v>MIL_UGA800_1007347_17855</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="F39" t="str">
-            <v>Uganda Military SNU</v>
-          </cell>
-          <cell r="G39" t="str">
-            <v>MIL_UGA800_000000000_17855</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="F40" t="str">
-            <v>UPDF 2nd Div.Hospital</v>
-          </cell>
-          <cell r="G40" t="str">
-            <v>MIL_UGA800_1004204_17855</v>
           </cell>
         </row>
       </sheetData>
@@ -1126,12 +817,12 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" customWidth="1"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="38.83203125" customWidth="1"/>
     <col min="3" max="3" width="35.83203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="15.83203125" style="3" customWidth="1"/>
@@ -1154,6 +845,12 @@
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
+      <c r="G1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="2" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1369,14 +1066,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
     <col min="2" max="2" width="38.83203125" customWidth="1"/>
     <col min="3" max="3" width="35.83203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="15.83203125" style="3" customWidth="1"/>
@@ -1399,6 +1096,12 @@
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
+      <c r="G1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="2" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1614,14 +1317,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
     <col min="2" max="2" width="38.83203125" customWidth="1"/>
     <col min="3" max="3" width="35.83203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="15.83203125" style="3" customWidth="1"/>
@@ -1644,6 +1347,12 @@
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
+      <c r="G1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="2" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>

</xml_diff>